<commit_message>
Debit: still missing tax calculation
</commit_message>
<xml_diff>
--- a/document/AELApp_GeneralDocument.xlsx
+++ b/document/AELApp_GeneralDocument.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\AEL\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="116">
   <si>
     <t>Module</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>Xuat hang</t>
+  </si>
+  <si>
+    <t>UI (reponsive table)</t>
   </si>
 </sst>
 </file>
@@ -568,6 +571,30 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -582,30 +609,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -908,14 +911,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -938,60 +941,60 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="27" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="25"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="26"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="27" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="26"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1083,99 +1086,99 @@
       <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
+      <c r="B16" s="22"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="23" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="23">
+      <c r="A21" s="16">
         <v>42157</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1184,11 +1187,11 @@
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1200,13 +1203,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="D14:H23"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:A20"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
@@ -1215,6 +1211,13 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D14:H23"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1225,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -1339,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,6 +1504,11 @@
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish accounting for debit/trans/exh
</commit_message>
<xml_diff>
--- a/document/AELApp_GeneralDocument.xlsx
+++ b/document/AELApp_GeneralDocument.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
   <si>
     <t>Module</t>
   </si>
@@ -213,12 +214,6 @@
     <t>some are not editable</t>
   </si>
   <si>
-    <t>find whole object at manager class</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
     <t>Docs</t>
   </si>
   <si>
@@ -249,51 +244,9 @@
     <t>database size modification</t>
   </si>
   <si>
-    <t>bug configuration edit form</t>
-  </si>
-  <si>
-    <t>format number</t>
-  </si>
-  <si>
     <t>inscrease tomcat memory Pergem</t>
   </si>
   <si>
-    <t>date formmater</t>
-  </si>
-  <si>
-    <t>tong chi phi theo tung loai</t>
-  </si>
-  <si>
-    <t>select2</t>
-  </si>
-  <si>
-    <t>datatable</t>
-  </si>
-  <si>
-    <t>nestedtable</t>
-  </si>
-  <si>
-    <t>pnotify</t>
-  </si>
-  <si>
-    <t>reflowtable</t>
-  </si>
-  <si>
-    <t>boostwatch</t>
-  </si>
-  <si>
-    <t>webjars</t>
-  </si>
-  <si>
-    <t>datepicker</t>
-  </si>
-  <si>
-    <t>date-timepicker</t>
-  </si>
-  <si>
-    <t>fontawesome</t>
-  </si>
-  <si>
     <t> Chi phi Theo  tung lo  hang , tung khach hang theo thoi gian   ( vi du  thang 1, or  3thang) …</t>
   </si>
   <si>
@@ -309,15 +262,9 @@
     <t>-          San  luong tong hop cua tung loai hinh  dich vu hang thang or theo  thoi gian  minh can chon   </t>
   </si>
   <si>
-    <t>datetime format on UI</t>
-  </si>
-  <si>
     <t>san luong? Doanh thu?</t>
   </si>
   <si>
-    <t>add new when not match</t>
-  </si>
-  <si>
     <t>Ngày giao hàng</t>
   </si>
   <si>
@@ -345,61 +292,85 @@
     <t>*Thoi gian tinh bang field nao</t>
   </si>
   <si>
-    <t>DEBIT</t>
-  </si>
-  <si>
-    <t>finish ui + excel</t>
-  </si>
-  <si>
-    <t>Trans</t>
-  </si>
-  <si>
-    <t>finish UI + excel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Profit load </t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>Excel</t>
-  </si>
-  <si>
-    <t>accounting fee tables</t>
-  </si>
-  <si>
-    <t>workflow (detail)</t>
-  </si>
-  <si>
     <t>Trucking</t>
   </si>
   <si>
-    <t>Fee details</t>
-  </si>
-  <si>
-    <t>Debit UI</t>
-  </si>
-  <si>
-    <t>Trans UI</t>
-  </si>
-  <si>
-    <t>Profit Load UI</t>
-  </si>
-  <si>
-    <t>Accounting fee tables</t>
-  </si>
-  <si>
-    <t>Workflow</t>
-  </si>
-  <si>
-    <t>Nhap hang</t>
-  </si>
-  <si>
-    <t>Xuat hang</t>
-  </si>
-  <si>
-    <t>UI (reponsive table)</t>
+    <t>attach file bao gia</t>
+  </si>
+  <si>
+    <t>cho accounting xem luc nhap thong tin</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>thong tin hai quan</t>
+  </si>
+  <si>
+    <t>import  from excel</t>
+  </si>
+  <si>
+    <t>attach files PDF</t>
+  </si>
+  <si>
+    <t>all services</t>
+  </si>
+  <si>
+    <t>ngay hang den = mien phi luu cong den + ngay</t>
+  </si>
+  <si>
+    <t>cho phep in bien bang giao hang</t>
+  </si>
+  <si>
+    <t>bang ke nha thau</t>
+  </si>
+  <si>
+    <t>nha thau: filter: khach hang, jobno, time (cho 1 nha thau)</t>
+  </si>
+  <si>
+    <t>tam ung: nhan vien/ke toan input</t>
+  </si>
+  <si>
+    <t>chi: hoan ung/ chi tien mat</t>
+  </si>
+  <si>
+    <t>ke toan(level) =&gt; chi phi duyet</t>
+  </si>
+  <si>
+    <t>chi phi =&gt; ke toan duyet =&gt; duyet chi phi</t>
+  </si>
+  <si>
+    <t>Tam ung</t>
+  </si>
+  <si>
+    <t>profil</t>
+  </si>
+  <si>
+    <t>Import Sales</t>
+  </si>
+  <si>
+    <t>Update data</t>
+  </si>
+  <si>
+    <t>in bao gia</t>
+  </si>
+  <si>
+    <t>in bien ban giao hang</t>
+  </si>
+  <si>
+    <t>link lan nhau cho tat ca cac list (new tab)</t>
+  </si>
+  <si>
+    <t>decorate button with icon</t>
+  </si>
+  <si>
+    <t>delete TEST data</t>
+  </si>
+  <si>
+    <t>chi phi trucking co duyet ko</t>
+  </si>
+  <si>
+    <t>profit load</t>
   </si>
 </sst>
 </file>
@@ -571,30 +542,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -609,6 +556,30 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -895,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:B16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,14 +882,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -941,60 +912,60 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="19" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="20"/>
+      <c r="F4" s="25"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1086,99 +1057,99 @@
       <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="B16" s="27"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+      <c r="A21" s="23">
         <v>42157</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1187,11 +1158,11 @@
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1203,6 +1174,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D14:H23"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:A20"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
@@ -1211,13 +1189,6 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="D14:H23"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1226,14 +1197,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="6.140625" bestFit="1" customWidth="1"/>
@@ -1242,99 +1214,63 @@
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" t="s">
-        <v>107</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
       </c>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>97</v>
       </c>
       <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>98</v>
-      </c>
-      <c r="E2" s="13">
-        <v>42065</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13" t="s">
-        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="13">
-        <v>42066</v>
-      </c>
-      <c r="F3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
-      <c r="B4" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="13">
-        <v>42068</v>
-      </c>
-      <c r="E4" s="13">
-        <v>42067</v>
-      </c>
-      <c r="F4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="29"/>
-      <c r="C5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>105</v>
-      </c>
+      <c r="B4" s="13"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="29"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1342,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1289,7 @@
     <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1361,7 +1297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1369,7 +1305,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1377,7 +1313,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1385,7 +1321,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1393,17 +1329,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1411,7 +1347,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1422,93 +1358,67 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>69</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>115</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1538,22 +1448,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L2" s="14" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -1564,46 +1474,46 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1616,75 +1526,140 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="G12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merge export for sales
</commit_message>
<xml_diff>
--- a/document/AELApp_GeneralDocument.xlsx
+++ b/document/AELApp_GeneralDocument.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
   <si>
     <t>Module</t>
   </si>
@@ -247,75 +247,15 @@
     <t>inscrease tomcat memory Pergem</t>
   </si>
   <si>
-    <t> Chi phi Theo  tung lo  hang , tung khach hang theo thoi gian   ( vi du  thang 1, or  3thang) …</t>
-  </si>
-  <si>
-    <t>-          DOanh thu Theo  tung lo  hang , tung khach hang theo thoi gian   ( vi du  thang 1, or  3thang) …</t>
-  </si>
-  <si>
-    <t>-          Tong  hop  san luong  va   chi phi theo  tung NHA THAU , theo thang or theo khach hang, theo  job file   or theo  thoi gian  minh can  con</t>
-  </si>
-  <si>
-    <t>-          San luong cac lo hang cua tung khach hang  , hang thang or theo thoi gian minh can chon</t>
-  </si>
-  <si>
-    <t>-          San  luong tong hop cua tung loai hinh  dich vu hang thang or theo  thoi gian  minh can chon   </t>
-  </si>
-  <si>
-    <t>san luong? Doanh thu?</t>
-  </si>
-  <si>
-    <t>Ngày giao hàng</t>
-  </si>
-  <si>
-    <t>Tên chi phí</t>
-  </si>
-  <si>
-    <t>Loại chi phí</t>
-  </si>
-  <si>
-    <t>Loại dịch vụ</t>
-  </si>
-  <si>
-    <t>JobFile</t>
-  </si>
-  <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>Bảng chi phí</t>
-  </si>
-  <si>
-    <t>Thông tin khách hàng</t>
-  </si>
-  <si>
-    <t>*Thoi gian tinh bang field nao</t>
-  </si>
-  <si>
     <t>Trucking</t>
   </si>
   <si>
-    <t>attach file bao gia</t>
-  </si>
-  <si>
-    <t>cho accounting xem luc nhap thong tin</t>
-  </si>
-  <si>
-    <t>PDF</t>
-  </si>
-  <si>
     <t>thong tin hai quan</t>
   </si>
   <si>
     <t>import  from excel</t>
   </si>
   <si>
-    <t>attach files PDF</t>
-  </si>
-  <si>
-    <t>all services</t>
-  </si>
-  <si>
     <t>ngay hang den = mien phi luu cong den + ngay</t>
   </si>
   <si>
@@ -340,12 +280,6 @@
     <t>chi phi =&gt; ke toan duyet =&gt; duyet chi phi</t>
   </si>
   <si>
-    <t>Tam ung</t>
-  </si>
-  <si>
-    <t>profil</t>
-  </si>
-  <si>
     <t>Import Sales</t>
   </si>
   <si>
@@ -371,13 +305,43 @@
   </si>
   <si>
     <t>profit load</t>
+  </si>
+  <si>
+    <t>Sealand</t>
+  </si>
+  <si>
+    <t>FCL nocont table</t>
+  </si>
+  <si>
+    <t>2. Sealand LCL có bang CONT hay ko?</t>
+  </si>
+  <si>
+    <t>1. Hàng nhap/xuat thi sao?</t>
+  </si>
+  <si>
+    <t>Hoàn thành thủ tục hản quan _ hightlight</t>
+  </si>
+  <si>
+    <t>attachment</t>
+  </si>
+  <si>
+    <t>Bo sung  noi giao hang cho tung containe</t>
+  </si>
+  <si>
+    <t>trucking</t>
+  </si>
+  <si>
+    <t>max size for pdf attachment</t>
+  </si>
+  <si>
+    <t>add logger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,12 +407,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -519,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -536,12 +494,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -556,30 +534,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -882,14 +836,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -912,60 +866,60 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="25"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="26"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="25" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="26"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1057,99 +1011,99 @@
       <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
+      <c r="B16" s="20"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="23">
+      <c r="A21" s="14">
         <v>42157</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1158,11 +1112,11 @@
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1174,13 +1128,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="D14:H23"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:A20"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
@@ -1189,6 +1136,13 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D14:H23"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1218,55 +1172,55 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="13"/>
+        <v>77</v>
+      </c>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>98</v>
+      <c r="B3" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="13"/>
+        <v>78</v>
+      </c>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="A5" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="B6" s="27"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="27"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1280,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,6 +1317,11 @@
         <v>54</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>55</v>
@@ -1401,6 +1360,11 @@
         <v>62</v>
       </c>
     </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+    </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>63</v>
@@ -1408,17 +1372,17 @@
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1429,107 +1393,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="63.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L2" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="33" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="33" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:H5"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A4:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,22 +1420,6 @@
     <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>82</v>
-      </c>
-    </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
@@ -1562,76 +1427,68 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
+      <c r="B9" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
+      <c r="B19" s="13"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
+      <c r="B23" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1641,22 +1498,46 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Update trucking detail - Fix report bug for sales
</commit_message>
<xml_diff>
--- a/document/AELApp_GeneralDocument.xlsx
+++ b/document/AELApp_GeneralDocument.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
   <si>
     <t>Module</t>
   </si>
@@ -307,15 +307,6 @@
     <t>profit load</t>
   </si>
   <si>
-    <t>Sealand</t>
-  </si>
-  <si>
-    <t>FCL nocont table</t>
-  </si>
-  <si>
-    <t>2. Sealand LCL có bang CONT hay ko?</t>
-  </si>
-  <si>
     <t>1. Hàng nhap/xuat thi sao?</t>
   </si>
   <si>
@@ -325,16 +316,31 @@
     <t>attachment</t>
   </si>
   <si>
-    <t>Bo sung  noi giao hang cho tung containe</t>
-  </si>
-  <si>
-    <t>trucking</t>
-  </si>
-  <si>
     <t>max size for pdf attachment</t>
   </si>
   <si>
     <t>add logger</t>
+  </si>
+  <si>
+    <t>0000 for auto gen</t>
+  </si>
+  <si>
+    <t>LCL -&gt; add -&gt; FCL :bug</t>
+  </si>
+  <si>
+    <t>4. Hoi lai phieu de nghi thanh toan</t>
+  </si>
+  <si>
+    <t>5. Phieu thu chi ouref</t>
+  </si>
+  <si>
+    <t>refund cho 1 job???</t>
+  </si>
+  <si>
+    <t>6. Ke hoach van tai</t>
+  </si>
+  <si>
+    <t>7. Container template</t>
   </si>
 </sst>
 </file>
@@ -1232,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,7 +1249,7 @@
     <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1267,7 +1273,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1275,7 +1281,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1283,17 +1289,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1301,7 +1307,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1312,22 +1318,25 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="F13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>56</v>
       </c>
@@ -1342,6 +1351,11 @@
         <v>58</v>
       </c>
     </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>59</v>
@@ -1362,7 +1376,7 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -1498,46 +1512,50 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A4:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>85</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Xuat/Nhap for Thong quan
</commit_message>
<xml_diff>
--- a/document/AELApp_GeneralDocument.xlsx
+++ b/document/AELApp_GeneralDocument.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
   <si>
     <t>Module</t>
   </si>
@@ -286,9 +286,6 @@
     <t>Update data</t>
   </si>
   <si>
-    <t>in bao gia</t>
-  </si>
-  <si>
     <t>in bien ban giao hang</t>
   </si>
   <si>
@@ -307,10 +304,7 @@
     <t>profit load</t>
   </si>
   <si>
-    <t>1. Hàng nhap/xuat thi sao?</t>
-  </si>
-  <si>
-    <t>Hoàn thành thủ tục hản quan _ hightlight</t>
+    <t>Sealand</t>
   </si>
   <si>
     <t>attachment</t>
@@ -341,6 +335,24 @@
   </si>
   <si>
     <t>7. Container template</t>
+  </si>
+  <si>
+    <t>Import data</t>
+  </si>
+  <si>
+    <t>Tạm ứng</t>
+  </si>
+  <si>
+    <t>Rework</t>
+  </si>
+  <si>
+    <t>Inland</t>
+  </si>
+  <si>
+    <t>Thong quan</t>
+  </si>
+  <si>
+    <t>khong cho doi</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1172,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,9 +1196,6 @@
       <c r="B2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,7 +1206,7 @@
         <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -1238,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,7 +1258,7 @@
     <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1257,7 +1266,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1265,7 +1274,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1273,7 +1282,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1289,17 +1298,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1307,7 +1316,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1318,25 +1327,28 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="I13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>56</v>
       </c>
@@ -1353,7 +1365,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -1376,7 +1388,7 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -1386,17 +1398,17 @@
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1407,14 +1419,46 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1490,7 +1534,7 @@
         <v>70</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1498,7 +1542,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1512,50 +1556,42 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H19"/>
+  <dimension ref="E5:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Update task planning
</commit_message>
<xml_diff>
--- a/document/AELApp_GeneralDocument.xlsx
+++ b/document/AELApp_GeneralDocument.xlsx
@@ -9,17 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
   <si>
     <t>Module</t>
   </si>
@@ -208,9 +207,6 @@
     <t>some are not editable</t>
   </si>
   <si>
-    <t>Docs</t>
-  </si>
-  <si>
     <t>date time format on UI</t>
   </si>
   <si>
@@ -235,9 +231,6 @@
     <t>inscrease tomcat memory Pergem</t>
   </si>
   <si>
-    <t>Trucking</t>
-  </si>
-  <si>
     <t>thong tin hai quan</t>
   </si>
   <si>
@@ -268,15 +261,6 @@
     <t>chi phi =&gt; ke toan duyet =&gt; duyet chi phi</t>
   </si>
   <si>
-    <t>Import Sales</t>
-  </si>
-  <si>
-    <t>Update data</t>
-  </si>
-  <si>
-    <t>in bien ban giao hang</t>
-  </si>
-  <si>
     <t>link lan nhau cho tat ca cac list (new tab)</t>
   </si>
   <si>
@@ -286,18 +270,12 @@
     <t>delete TEST data</t>
   </si>
   <si>
-    <t>chi phi trucking co duyet ko</t>
-  </si>
-  <si>
     <t>profit load</t>
   </si>
   <si>
     <t>Sealand</t>
   </si>
   <si>
-    <t>attachment</t>
-  </si>
-  <si>
     <t>max size for pdf attachment</t>
   </si>
   <si>
@@ -307,24 +285,6 @@
     <t>LCL -&gt; add -&gt; FCL :bug</t>
   </si>
   <si>
-    <t>4. Hoi lai phieu de nghi thanh toan</t>
-  </si>
-  <si>
-    <t>5. Phieu thu chi ouref</t>
-  </si>
-  <si>
-    <t>refund cho 1 job???</t>
-  </si>
-  <si>
-    <t>6. Ke hoach van tai</t>
-  </si>
-  <si>
-    <t>7. Container template</t>
-  </si>
-  <si>
-    <t>Import data</t>
-  </si>
-  <si>
     <t>Tạm ứng</t>
   </si>
   <si>
@@ -341,6 +301,33 @@
   </si>
   <si>
     <t>UI icons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Reject </t>
+  </si>
+  <si>
+    <t>Import bang ke hai quan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Update </t>
+  </si>
+  <si>
+    <t>Thong quan &amp; Van Tai &amp; Trucking</t>
+  </si>
+  <si>
+    <t>3. Import cont seal</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Verify Modification - Testing</t>
+  </si>
+  <si>
+    <t>Profit load</t>
+  </si>
+  <si>
+    <t>Shipment Control</t>
   </si>
 </sst>
 </file>
@@ -483,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -500,32 +487,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,9 +503,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,14 +826,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -872,60 +856,60 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1017,99 +1001,99 @@
       <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
+      <c r="B16" s="24"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+      <c r="A21" s="20">
         <v>42157</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1118,11 +1102,11 @@
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1134,6 +1118,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D14:H23"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:A20"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
@@ -1142,13 +1133,6 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="D14:H23"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1157,87 +1141,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="27"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:B7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1293,7 +1199,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1309,73 +1215,73 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" t="s">
         <v>81</v>
-      </c>
-      <c r="F13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1384,13 +1290,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1399,30 +1303,25 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>91</v>
-      </c>
       <c r="B3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1430,12 +1329,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H23"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,75 +1344,67 @@
     <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>51</v>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="B5" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>64</v>
       </c>
-      <c r="H7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="G12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="13"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1521,44 +1412,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E5:H19"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="H15" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="H16" t="s">
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="26">
+        <v>42128</v>
+      </c>
+      <c r="J1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
+      <c r="B2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H18" t="s">
+      <c r="I2" s="26">
+        <v>42159</v>
+      </c>
+      <c r="J2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H19" t="s">
-        <v>88</v>
+      <c r="I3" s="26">
+        <v>42189</v>
+      </c>
+      <c r="J3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>